<commit_message>
New Files to new Branch
</commit_message>
<xml_diff>
--- a/resources/automation.xlsx
+++ b/resources/automation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pshende\OneDrive - Rythmos Inc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AppiumScene\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6576C20-D5F9-4728-965B-E8BD9C8B300A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ED1832-04F3-4221-A6EA-66825561078F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="7270" xr2:uid="{E01B78D0-CE4B-42B0-AB43-F6357D11EA7A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E01B78D0-CE4B-42B0-AB43-F6357D11EA7A}"/>
   </bookViews>
   <sheets>
     <sheet name="protractor" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>